<commit_message>
Hour rounds off now.
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572419555" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572419555" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572419555" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572419555"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572419852" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572419852" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572419852" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572419852"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Feature #</t>
   </si>
@@ -57,14 +57,16 @@
   </si>
   <si>
     <t>manifest entry - android:name=".CustomClasses.taskQGlobal"
-((taskQGlobal) getApplication()).bClearUserEntryNew()</t>
+((taskQGlobal) getApplication()).</t>
   </si>
   <si>
     <t>Tags Dialog to load the tags.</t>
   </si>
   <si>
-    <t xml:space="preserve">7
-</t>
+    <t>User Entry- Init of New Entry</t>
+  </si>
+  <si>
+    <t>Task entry form</t>
   </si>
 </sst>
 </file>
@@ -81,7 +83,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₹&quot;_-;\-* #,##0.00\ &quot;₹&quot;_-;_-* &quot;-&quot;??\ &quot;₹&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₹_-;\-* #,##0.00\ _₹_-;_-* &quot;-&quot;??\ _₹_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -89,7 +91,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572419555" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572419852" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -104,7 +106,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572419555" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572419852" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -115,41 +117,11 @@
     <font>
       <name val="Bitstream Vera Sans Mono"/>
       <family val="1"/>
-      <color rgb="FFA8C023"/>
+      <color rgb="FF7F7F7F"/>
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572419555" fgClr="A8C023" bgClr="A9B7C6" ulstyle="none">
-            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
-            <pm:cs face="Basic Sans" sz="180" lang="default"/>
-            <pm:ea face="Basic Sans" sz="180" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Bitstream Vera Sans Mono"/>
-      <family val="1"/>
-      <color rgb="FF6A8759"/>
-      <sz val="9"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572419555" fgClr="6A8759" bgClr="A9B7C6" ulstyle="none">
-            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
-            <pm:cs face="Basic Sans" sz="180" lang="default"/>
-            <pm:ea face="Basic Sans" sz="180" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Bitstream Vera Sans Mono"/>
-      <family val="1"/>
-      <color rgb="FFA9B7C6"/>
-      <sz val="9"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572419555" fgClr="A9B7C6" bgClr="A9B7C6" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572419852" fgClr="7F7F7F" bgClr="A9B7C6" ulstyle="none">
             <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
             <pm:cs face="Basic Sans" sz="180" lang="default"/>
             <pm:ea face="Basic Sans" sz="180" lang="default"/>
@@ -171,7 +143,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572419555" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572419852" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -193,7 +165,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572419555"/>
+          <pm:border xmlns:pm="smNativeData" id="1572419852"/>
         </ext>
       </extLst>
     </border>
@@ -212,7 +184,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572419555"/>
+          <pm:border xmlns:pm="smNativeData" id="1572419852"/>
         </ext>
       </extLst>
     </border>
@@ -232,10 +204,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572419555" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572419852" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572419555" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572419852" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -503,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D11"/>
+  <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -595,17 +567,25 @@
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572419555" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572419852" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -614,14 +594,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572419555" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572419555" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572419852" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572419852" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572419555" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572419852" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Date and Time pickers enabled.
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572419852" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572419852" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572419852" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572419852"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572423344" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572423344" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572423344" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572423344"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Feature #</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Task entry form</t>
+  </si>
+  <si>
+    <t>Allow the user to change the Date and Time the Task is Due</t>
   </si>
 </sst>
 </file>
@@ -91,7 +94,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572419852" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572423344" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -106,7 +109,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572419852" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572423344" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -117,12 +120,13 @@
     <font>
       <name val="Bitstream Vera Sans Mono"/>
       <family val="1"/>
-      <color rgb="FF7F7F7F"/>
+      <i/>
+      <color rgb="FFA8C023"/>
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572419852" fgClr="7F7F7F" bgClr="A9B7C6" ulstyle="none">
-            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
+          <pm:charSpec xmlns:pm="smNativeData" id="1572423344" fgClr="A8C023" bgClr="A9B7C6" ulstyle="none">
+            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default" i="1"/>
             <pm:cs face="Basic Sans" sz="180" lang="default"/>
             <pm:ea face="Basic Sans" sz="180" lang="default"/>
           </pm:charSpec>
@@ -143,7 +147,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572419852" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572423344" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -165,7 +169,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572419852"/>
+          <pm:border xmlns:pm="smNativeData" id="1572423344"/>
         </ext>
       </extLst>
     </border>
@@ -184,7 +188,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572419852"/>
+          <pm:border xmlns:pm="smNativeData" id="1572423344"/>
         </ext>
       </extLst>
     </border>
@@ -204,10 +208,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572419852" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572423344" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572419852" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572423344" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -475,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D12"/>
+  <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -581,11 +585,19 @@
         <v>13</v>
       </c>
     </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572419852" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572423344" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -594,14 +606,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572419852" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572419852" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572423344" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572423344" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572419852" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572423344" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Added the main dB and can now store new entries into main dB
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572423344" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572423344" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572423344" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572423344"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572428053" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572428053" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572428053" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572428053"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Feature #</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Allow the user to change the Date and Time the Task is Due</t>
+  </si>
+  <si>
+    <t>Main database of all entries</t>
+  </si>
+  <si>
+    <t>Save the form to the dBase. checks locally if it's a edit or a new entry</t>
   </si>
 </sst>
 </file>
@@ -86,7 +92,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₹&quot;_-;\-* #,##0.00\ &quot;₹&quot;_-;_-* &quot;-&quot;??\ &quot;₹&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₹_-;\-* #,##0.00\ _₹_-;_-* &quot;-&quot;??\ _₹_-;_-@_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -94,7 +100,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572423344" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572428053" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -109,26 +115,10 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572423344" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572428053" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Bitstream Vera Sans Mono"/>
-      <family val="1"/>
-      <i/>
-      <color rgb="FFA8C023"/>
-      <sz val="9"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572423344" fgClr="A8C023" bgClr="A9B7C6" ulstyle="none">
-            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default" i="1"/>
-            <pm:cs face="Basic Sans" sz="180" lang="default"/>
-            <pm:ea face="Basic Sans" sz="180" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -147,7 +137,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572423344" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572428053" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -169,7 +159,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572423344"/>
+          <pm:border xmlns:pm="smNativeData" id="1572428053"/>
         </ext>
       </extLst>
     </border>
@@ -188,7 +178,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572423344"/>
+          <pm:border xmlns:pm="smNativeData" id="1572428053"/>
         </ext>
       </extLst>
     </border>
@@ -208,10 +198,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572423344" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572428053" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572423344" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572428053" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -479,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -593,11 +583,27 @@
         <v>14</v>
       </c>
     </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572423344" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572428053" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -606,14 +612,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572423344" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572423344" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572428053" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572428053" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572423344" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572428053" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Basic list view implemented.
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572428053" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572428053" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572428053" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572428053"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572435815" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572435815" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572435815" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572435815"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Feature #</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Save the form to the dBase. checks locally if it's a edit or a new entry</t>
+  </si>
+  <si>
+    <t>List of all entries</t>
+  </si>
+  <si>
+    <t>additional shared assetts in listview_userentries.xml</t>
+  </si>
+  <si>
+    <t>Hide closed items</t>
   </si>
 </sst>
 </file>
@@ -92,7 +101,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₹&quot;_-;\-* #,##0.00\ &quot;₹&quot;_-;_-* &quot;-&quot;??\ &quot;₹&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₹_-;\-* #,##0.00\ _₹_-;_-* &quot;-&quot;??\ _₹_-;_-@_-"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -100,7 +109,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572428053" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572435815" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -115,10 +124,25 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572428053" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572435815" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Bitstream Vera Sans Mono"/>
+      <family val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="9"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572435815" fgClr="7F7F7F" bgClr="A9B7C6" ulstyle="none">
+            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
+            <pm:cs face="Basic Sans" sz="180" lang="default"/>
+            <pm:ea face="Basic Sans" sz="180" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -137,7 +161,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572428053" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572435815" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -159,7 +183,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572428053"/>
+          <pm:border xmlns:pm="smNativeData" id="1572435815"/>
         </ext>
       </extLst>
     </border>
@@ -178,7 +202,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572428053"/>
+          <pm:border xmlns:pm="smNativeData" id="1572435815"/>
         </ext>
       </extLst>
     </border>
@@ -186,8 +210,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -198,10 +225,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572428053" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572435815" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572428053" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572435815" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -469,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D15"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -599,11 +626,30 @@
         <v>16</v>
       </c>
     </row>
+    <row r="16" spans="2:4">
+      <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572428053" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572435815" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -612,14 +658,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572428053" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572428053" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572435815" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572435815" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572428053" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572435815" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
List View - All implemented
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572435815" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572435815" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572435815" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572435815"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572456941" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572456941" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572456941" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572456941"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Feature #</t>
   </si>
@@ -85,6 +85,17 @@
   </si>
   <si>
     <t>Hide closed items</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Listviews are cropped at the top and bottom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add a top padding to the listviews of taskQ_dialog_padding (16dp)
+add a bottom padding to the listviews of tapp_icon_size (48dp), which must be same as hight of tab_Button_NewItem button
+</t>
   </si>
 </sst>
 </file>
@@ -101,7 +112,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₹&quot;_-;\-* #,##0.00\ &quot;₹&quot;_-;_-* &quot;-&quot;??\ &quot;₹&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₹_-;\-* #,##0.00\ _₹_-;_-* &quot;-&quot;??\ _₹_-;_-@_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -109,7 +120,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572435815" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572456941" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -124,25 +135,10 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572435815" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572456941" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Bitstream Vera Sans Mono"/>
-      <family val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="9"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572435815" fgClr="7F7F7F" bgClr="A9B7C6" ulstyle="none">
-            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
-            <pm:cs face="Basic Sans" sz="180" lang="default"/>
-            <pm:ea face="Basic Sans" sz="180" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -161,7 +157,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572435815" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572456941" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -183,7 +179,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572435815"/>
+          <pm:border xmlns:pm="smNativeData" id="1572456941"/>
         </ext>
       </extLst>
     </border>
@@ -202,7 +198,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572435815"/>
+          <pm:border xmlns:pm="smNativeData" id="1572456941"/>
         </ext>
       </extLst>
     </border>
@@ -225,10 +221,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572435815" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572456941" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572435815" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572456941" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -496,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D17"/>
+  <dimension ref="B2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -633,7 +629,7 @@
       <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -643,13 +639,24 @@
       </c>
       <c r="C17" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572435815" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572456941" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -658,14 +665,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572435815" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572435815" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572456941" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572456941" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572435815" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572456941" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
List View - All can now be used to edit tasks. Tags pending.
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572456941" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572456941" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572456941" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572456941"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572497685" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572497685" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572497685" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572497685"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Feature #</t>
   </si>
@@ -96,6 +96,12 @@
     <t xml:space="preserve">add a top padding to the listviews of taskQ_dialog_padding (16dp)
 add a bottom padding to the listviews of tapp_icon_size (48dp), which must be same as hight of tab_Button_NewItem button
 </t>
+  </si>
+  <si>
+    <t>Allow items to be opened for the All-Fragment</t>
+  </si>
+  <si>
+    <t>User Entry- Modify existing Entry</t>
   </si>
 </sst>
 </file>
@@ -112,7 +118,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₹&quot;_-;\-* #,##0.00\ &quot;₹&quot;_-;_-* &quot;-&quot;??\ &quot;₹&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₹_-;\-* #,##0.00\ _₹_-;_-* &quot;-&quot;??\ _₹_-;_-@_-"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -120,7 +126,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572456941" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572497685" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -135,10 +141,25 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572456941" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572497685" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Bitstream Vera Sans Mono"/>
+      <family val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="9"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572497685" fgClr="7F7F7F" bgClr="A9B7C6" ulstyle="none">
+            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
+            <pm:cs face="Basic Sans" sz="180" lang="default"/>
+            <pm:ea face="Basic Sans" sz="180" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -157,7 +178,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572456941" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572497685" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -179,7 +200,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572456941"/>
+          <pm:border xmlns:pm="smNativeData" id="1572497685"/>
         </ext>
       </extLst>
     </border>
@@ -198,7 +219,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572456941"/>
+          <pm:border xmlns:pm="smNativeData" id="1572497685"/>
         </ext>
       </extLst>
     </border>
@@ -206,11 +227,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -221,10 +239,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572456941" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572497685" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572456941" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572497685" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -492,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D18"/>
+  <dimension ref="B2:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -648,15 +666,31 @@
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="n">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="n">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572456941" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572497685" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -665,14 +699,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572456941" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572456941" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572497685" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572497685" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572456941" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572497685" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
What fragment implemented with formatting errors
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572497685" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572497685" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572497685" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572497685"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572507515" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572507515" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572507515" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572507515"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Feature #</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>User Entry- Modify existing Entry</t>
+  </si>
+  <si>
+    <t>Create a dBase of only tags</t>
   </si>
 </sst>
 </file>
@@ -118,7 +121,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₹&quot;_-;\-* #,##0.00\ &quot;₹&quot;_-;_-* &quot;-&quot;??\ &quot;₹&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₹_-;\-* #,##0.00\ _₹_-;_-* &quot;-&quot;??\ _₹_-;_-@_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -126,7 +129,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572497685" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572507515" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -141,25 +144,10 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572497685" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572507515" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Bitstream Vera Sans Mono"/>
-      <family val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="9"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572497685" fgClr="7F7F7F" bgClr="A9B7C6" ulstyle="none">
-            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
-            <pm:cs face="Basic Sans" sz="180" lang="default"/>
-            <pm:ea face="Basic Sans" sz="180" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -178,7 +166,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572497685" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572507515" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -200,7 +188,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572497685"/>
+          <pm:border xmlns:pm="smNativeData" id="1572507515"/>
         </ext>
       </extLst>
     </border>
@@ -219,7 +207,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572497685"/>
+          <pm:border xmlns:pm="smNativeData" id="1572507515"/>
         </ext>
       </extLst>
     </border>
@@ -239,10 +227,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572497685" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572507515" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572497685" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572507515" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -510,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D20"/>
+  <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -686,11 +674,19 @@
         <v>24</v>
       </c>
     </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="n">
+        <v>18</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572497685" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572507515" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -699,14 +695,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572497685" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572497685" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572507515" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572507515" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572497685" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572507515" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Tasks can now be deleted
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572507515" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572507515" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572507515" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572507515"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572545884" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572545884" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572545884" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572545884"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Feature #</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Create a dBase of only tags</t>
+  </si>
+  <si>
+    <t>Allow user to delete tasks permanently</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572507515" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572545884" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -144,7 +147,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572507515" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572545884" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -166,7 +169,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572507515" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572545884" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -188,7 +191,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572507515"/>
+          <pm:border xmlns:pm="smNativeData" id="1572545884"/>
         </ext>
       </extLst>
     </border>
@@ -207,7 +210,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572507515"/>
+          <pm:border xmlns:pm="smNativeData" id="1572545884"/>
         </ext>
       </extLst>
     </border>
@@ -227,10 +230,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572507515" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572545884" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572507515" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572545884" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -498,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D21"/>
+  <dimension ref="B2:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -682,11 +685,19 @@
         <v>25</v>
       </c>
     </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="n">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572507515" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572545884" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -695,14 +706,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572507515" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572507515" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572545884" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572545884" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572507515" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572545884" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Added the Time dBase Arch and Manager
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572545884" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572545884" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572545884" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572545884"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572577063" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572577063" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572577063" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572577063"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Feature #</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Allow user to delete tasks permanently</t>
+  </si>
+  <si>
+    <t>Create a dBase based on Time</t>
   </si>
 </sst>
 </file>
@@ -132,7 +135,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572545884" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572577063" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -147,7 +150,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572545884" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572577063" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -169,7 +172,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572545884" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572577063" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -191,7 +194,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572545884"/>
+          <pm:border xmlns:pm="smNativeData" id="1572577063"/>
         </ext>
       </extLst>
     </border>
@@ -210,7 +213,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572545884"/>
+          <pm:border xmlns:pm="smNativeData" id="1572577063"/>
         </ext>
       </extLst>
     </border>
@@ -230,10 +233,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572545884" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572577063" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572545884" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572577063" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -501,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D22"/>
+  <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -693,11 +696,19 @@
         <v>26</v>
       </c>
     </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="n">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572545884" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572577063" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -706,14 +717,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572545884" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572545884" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572577063" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572577063" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572545884" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572577063" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
//Feature - 21 Comfort edit dates implemented
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572577063" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572577063" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572577063" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572577063"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572584933" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572584933" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572584933" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572584933"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Feature #</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Create a dBase based on Time</t>
+  </si>
+  <si>
+    <t>Comfort edit dates</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572577063" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572584933" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -150,7 +153,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572577063" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572584933" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -172,7 +175,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572577063" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572584933" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -194,7 +197,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572577063"/>
+          <pm:border xmlns:pm="smNativeData" id="1572584933"/>
         </ext>
       </extLst>
     </border>
@@ -213,7 +216,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572577063"/>
+          <pm:border xmlns:pm="smNativeData" id="1572584933"/>
         </ext>
       </extLst>
     </border>
@@ -233,10 +236,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572577063" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572584933" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572577063" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572584933" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -504,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D23"/>
+  <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -704,11 +707,19 @@
         <v>27</v>
       </c>
     </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="n">
+        <v>21</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572577063" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572584933" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -717,14 +728,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572577063" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572577063" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572584933" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572584933" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572577063" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572584933" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
//Feature - 22 Contacts in user entry dialog
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572584933" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572584933" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572584933" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572584933"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572585086" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572585086" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572585086" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572585086"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Feature #</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Comfort edit dates</t>
+  </si>
+  <si>
+    <t>Contacts in user entry dialog</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572584933" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572585086" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -153,7 +156,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572584933" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572585086" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -175,7 +178,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572584933" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572585086" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -197,7 +200,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572584933"/>
+          <pm:border xmlns:pm="smNativeData" id="1572585086"/>
         </ext>
       </extLst>
     </border>
@@ -216,7 +219,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572584933"/>
+          <pm:border xmlns:pm="smNativeData" id="1572585086"/>
         </ext>
       </extLst>
     </border>
@@ -236,10 +239,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572584933" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572585086" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572584933" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572585086" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -507,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D24"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
@@ -715,11 +718,19 @@
         <v>28</v>
       </c>
     </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="n">
+        <v>22</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572584933" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572585086" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -728,14 +739,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572584933" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572584933" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572585086" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572585086" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572584933" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572585086" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Basic Notification functionality implemented
</commit_message>
<xml_diff>
--- a/Doc/taskQv2.Documentation.xlsx
+++ b/Doc/taskQv2.Documentation.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572606543" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572606543" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572606543" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572606543"/>
+      <pm:revision xmlns:pm="smNativeData" day="1572609550" val="971" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1572609550" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1572609550" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1572609550"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Feature #</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Notifications</t>
+  </si>
+  <si>
+    <t>Added 4 files to services folder
+Added receiverNotification and receiverNotificationAction to the manifest
+Added RECEIVE_BOOT_COMPLETED permission
+Registered channel in main activity OnCreate</t>
   </si>
 </sst>
 </file>
@@ -136,7 +142,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₹&quot;_-;\-* #,##0.00\ &quot;₹&quot;_-;_-* &quot;-&quot;??\ &quot;₹&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₹_-;\-* #,##0.00\ _₹_-;_-* &quot;-&quot;??\ _₹_-;_-@_-"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -144,7 +150,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572606543" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572609550" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -159,10 +165,25 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572606543" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572609550" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Bitstream Vera Sans Mono"/>
+      <family val="1"/>
+      <color rgb="FFA8C023"/>
+      <sz val="9"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1572609550" fgClr="A8C023" bgClr="A9B7C6" ulstyle="none">
+            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
+            <pm:cs face="Basic Sans" sz="180" lang="default"/>
+            <pm:ea face="Basic Sans" sz="180" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -181,7 +202,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572606543" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1572609550" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -203,7 +224,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572606543"/>
+          <pm:border xmlns:pm="smNativeData" id="1572609550"/>
         </ext>
       </extLst>
     </border>
@@ -222,7 +243,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572606543"/>
+          <pm:border xmlns:pm="smNativeData" id="1572609550"/>
         </ext>
       </extLst>
     </border>
@@ -230,8 +251,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -242,10 +266,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572606543" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1572609550" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1572606543" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1572609550" count="5">
         <pm:color name="Color 26" rgb="A8C023"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -515,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -729,19 +753,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:4">
       <c r="B26" t="n">
         <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572606543" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1572609550" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -750,14 +777,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572606543" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572606543" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1572609550" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1572609550" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572606543" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572609550" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>